<commit_message>
added SMAs to fig 1 and more
</commit_message>
<xml_diff>
--- a/data/california/da_sampling/data/raw/bivalve_product_key.xlsx
+++ b/data/california/da_sampling/data/raw/bivalve_product_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/data/california/da_sampling/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C284FC0-8C8C-8042-A7FF-DA201EC89D24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D713F-DCEF-5046-9F4B-3AF80A547646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20720" yWindow="2980" windowWidth="28040" windowHeight="17440" xr2:uid="{C83B9E4C-1F72-8645-992D-A0D6828A020E}"/>
+    <workbookView xWindow="18820" yWindow="3040" windowWidth="28040" windowHeight="17440" xr2:uid="{C83B9E4C-1F72-8645-992D-A0D6828A020E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
   <si>
     <t>tissue</t>
   </si>
@@ -132,12 +132,6 @@
     <t>Rock scallop</t>
   </si>
   <si>
-    <t>Bay mussel</t>
-  </si>
-  <si>
-    <t>Sea mussel</t>
-  </si>
-  <si>
     <t>Barred surfperch</t>
   </si>
   <si>
@@ -150,343 +144,355 @@
     <t>Shiner surfperch</t>
   </si>
   <si>
+    <t>Pismo clam</t>
+  </si>
+  <si>
+    <t>Razor clam</t>
+  </si>
+  <si>
+    <t>Pacific oyster</t>
+  </si>
+  <si>
+    <t>Northern anchovy</t>
+  </si>
+  <si>
+    <t>Spiny lobster</t>
+  </si>
+  <si>
+    <t>Manila clam</t>
+  </si>
+  <si>
+    <t>California yellowtail</t>
+  </si>
+  <si>
+    <t>Pacific lamprey</t>
+  </si>
+  <si>
+    <t>Littleneck clam</t>
+  </si>
+  <si>
+    <t>Kumamoto oyster</t>
+  </si>
+  <si>
+    <t>Basket cockle</t>
+  </si>
+  <si>
+    <t>Red abalone</t>
+  </si>
+  <si>
+    <t>Surfperch, Barred, Meat</t>
+  </si>
+  <si>
+    <t>Surfperch, Barred, Viscera</t>
+  </si>
+  <si>
+    <t>Bay Mussel, cultured</t>
+  </si>
+  <si>
+    <t>Bay Mussel, wild</t>
+  </si>
+  <si>
+    <t>Surfperch, Black, Meat</t>
+  </si>
+  <si>
+    <t>Butter Clam</t>
+  </si>
+  <si>
+    <t>Gaper Clam meat</t>
+  </si>
+  <si>
+    <t>Gaper Clam viscera</t>
+  </si>
+  <si>
+    <t>Mackerel</t>
+  </si>
+  <si>
+    <t>Mackerel, muscle</t>
+  </si>
+  <si>
+    <t>Northern Anchovy, head</t>
+  </si>
+  <si>
+    <t>Northern Anchovy, meat</t>
+  </si>
+  <si>
+    <t>Lamprey, Pacific, meat</t>
+  </si>
+  <si>
+    <t>Pacific Oyster, cultured</t>
+  </si>
+  <si>
+    <t>Surfperch, Pile, Viscera</t>
+  </si>
+  <si>
+    <t>Pismo Clam</t>
+  </si>
+  <si>
+    <t>Razor Clam meat</t>
+  </si>
+  <si>
+    <t>Razor Clam viscera</t>
+  </si>
+  <si>
+    <t>Abalone, red</t>
+  </si>
+  <si>
+    <t>Abalone, red viscera</t>
+  </si>
+  <si>
+    <t>Cultured Rock Scallop, viscera</t>
+  </si>
+  <si>
+    <t>Rock Scallop viscera</t>
+  </si>
+  <si>
+    <t>Sardine, muscle</t>
+  </si>
+  <si>
+    <t>Sardine, viscera</t>
+  </si>
+  <si>
+    <t>Sardine, whole</t>
+  </si>
+  <si>
+    <t>Sea Mussel, Sentinel</t>
+  </si>
+  <si>
+    <t>Sea Mussel, wild</t>
+  </si>
+  <si>
+    <t>Surfperch, Shiner, Meat</t>
+  </si>
+  <si>
+    <t>Surfperch, Shiner, Viscera</t>
+  </si>
+  <si>
+    <t>Lobster, Spiny, muscle</t>
+  </si>
+  <si>
+    <t>Lobster, Spiny, viscera</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>comm_name</t>
+  </si>
+  <si>
+    <t>Mixed Sea/Bay Mussels</t>
+  </si>
+  <si>
+    <t>Washington Clam, siphon</t>
+  </si>
+  <si>
+    <t>Bay Mussel, Sentinel</t>
+  </si>
+  <si>
+    <t>Clam, unidentified</t>
+  </si>
+  <si>
+    <t>Salmon, meat</t>
+  </si>
+  <si>
+    <t>Salmon, liver</t>
+  </si>
+  <si>
+    <t>Salmon, viscera</t>
+  </si>
+  <si>
+    <t>Ray, Thornback, meat</t>
+  </si>
+  <si>
+    <t>Ray, Thornback, viscera</t>
+  </si>
+  <si>
+    <t>Grunion, whole</t>
+  </si>
+  <si>
+    <t>Gooseneck Barnacle</t>
+  </si>
+  <si>
+    <t>Pismo Clam muscle</t>
+  </si>
+  <si>
+    <t>Pismo Clam viscera</t>
+  </si>
+  <si>
+    <t>Rock Scallop, wild</t>
+  </si>
+  <si>
+    <t>Sea Otter Stomach Contents</t>
+  </si>
+  <si>
+    <t>Gaper Clam siphon</t>
+  </si>
+  <si>
+    <t>Matrix spike, mussel</t>
+  </si>
+  <si>
+    <t>Rock Scallop mantle, gills</t>
+  </si>
+  <si>
+    <t>Lobster, Spiny, roe</t>
+  </si>
+  <si>
+    <t>Thornback ray</t>
+  </si>
+  <si>
+    <t>Grunion</t>
+  </si>
+  <si>
+    <t>Gooseneck barnacle</t>
+  </si>
+  <si>
+    <t>Sea otter</t>
+  </si>
+  <si>
+    <t>siphon</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>liver</t>
+  </si>
+  <si>
+    <t>stomach contents</t>
+  </si>
+  <si>
+    <t>mantle/gills</t>
+  </si>
+  <si>
+    <t>roe</t>
+  </si>
+  <si>
+    <t>Clam spp.</t>
+  </si>
+  <si>
+    <t>Mussel spp.</t>
+  </si>
+  <si>
+    <t>matrix spike</t>
+  </si>
+  <si>
+    <t>Crab, Red Rock, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Dungeness, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Spider, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Brown Rock, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Pelagic Red</t>
+  </si>
+  <si>
+    <t>Pelagic Red Crab, tail</t>
+  </si>
+  <si>
+    <t>Pelagic Red Crab, head</t>
+  </si>
+  <si>
+    <t>Crab, Red Rock</t>
+  </si>
+  <si>
+    <t>Crab, unknown rock, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Yellow Rock, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Red Rock, body meat</t>
+  </si>
+  <si>
+    <t>Crab, Red Rock, leg meat</t>
+  </si>
+  <si>
+    <t>Crab, Yellow Rock, body meat</t>
+  </si>
+  <si>
+    <t>Crab, Yellow Rock, leg meat</t>
+  </si>
+  <si>
+    <t>Crab, Brown Rock, body meat</t>
+  </si>
+  <si>
+    <t>Crab, Brown Rock, leg meat</t>
+  </si>
+  <si>
+    <t>Crab, Dungeness, body meat</t>
+  </si>
+  <si>
+    <t>Crab, Dungeness, leg meat</t>
+  </si>
+  <si>
+    <t>Crab, unknown rock, body meat</t>
+  </si>
+  <si>
+    <t>Crab, Stone, viscera</t>
+  </si>
+  <si>
+    <t>Crab, Swimming</t>
+  </si>
+  <si>
+    <t>Red rock crab</t>
+  </si>
+  <si>
+    <t>Stone crab</t>
+  </si>
+  <si>
+    <t>Swimming crab</t>
+  </si>
+  <si>
+    <t>Rock crab</t>
+  </si>
+  <si>
+    <t>Yellow rock crab</t>
+  </si>
+  <si>
+    <t>Dungeness crab</t>
+  </si>
+  <si>
+    <t>Brown rock crab</t>
+  </si>
+  <si>
+    <t>Pelagic red crab</t>
+  </si>
+  <si>
+    <t>body meat</t>
+  </si>
+  <si>
+    <t>leg meat</t>
+  </si>
+  <si>
+    <t>tail</t>
+  </si>
+  <si>
+    <t>Pacific sardine</t>
+  </si>
+  <si>
+    <t>California market squid</t>
+  </si>
+  <si>
+    <t>Sheep (spider) crab</t>
+  </si>
+  <si>
+    <t>Gaper (horse) clam</t>
+  </si>
+  <si>
     <t>Washington clam</t>
   </si>
   <si>
-    <t>Pismo clam</t>
-  </si>
-  <si>
-    <t>Razor clam</t>
-  </si>
-  <si>
-    <t>Pacific oyster</t>
-  </si>
-  <si>
-    <t>Northern anchovy</t>
-  </si>
-  <si>
-    <t>Spiny lobster</t>
-  </si>
-  <si>
-    <t>Manila clam</t>
-  </si>
-  <si>
     <t>Butter clam</t>
   </si>
   <si>
-    <t>California yellowtail</t>
-  </si>
-  <si>
-    <t>Gaper clam</t>
-  </si>
-  <si>
-    <t>Pacific lamprey</t>
-  </si>
-  <si>
-    <t>Littleneck clam</t>
-  </si>
-  <si>
-    <t>Kumamoto oyster</t>
-  </si>
-  <si>
-    <t>Basket cockle</t>
-  </si>
-  <si>
-    <t>Red abalone</t>
-  </si>
-  <si>
-    <t>Surfperch, Barred, Meat</t>
-  </si>
-  <si>
-    <t>Surfperch, Barred, Viscera</t>
-  </si>
-  <si>
-    <t>Bay Mussel, cultured</t>
-  </si>
-  <si>
-    <t>Bay Mussel, wild</t>
-  </si>
-  <si>
-    <t>Surfperch, Black, Meat</t>
-  </si>
-  <si>
-    <t>Butter Clam</t>
-  </si>
-  <si>
-    <t>Gaper Clam meat</t>
-  </si>
-  <si>
-    <t>Gaper Clam viscera</t>
-  </si>
-  <si>
-    <t>Mackerel</t>
-  </si>
-  <si>
-    <t>Mackerel, muscle</t>
-  </si>
-  <si>
-    <t>Northern Anchovy, head</t>
-  </si>
-  <si>
-    <t>Northern Anchovy, meat</t>
-  </si>
-  <si>
-    <t>Lamprey, Pacific, meat</t>
-  </si>
-  <si>
-    <t>Pacific Oyster, cultured</t>
-  </si>
-  <si>
-    <t>Surfperch, Pile, Viscera</t>
-  </si>
-  <si>
-    <t>Pismo Clam</t>
-  </si>
-  <si>
-    <t>Razor Clam meat</t>
-  </si>
-  <si>
-    <t>Razor Clam viscera</t>
-  </si>
-  <si>
-    <t>Abalone, red</t>
-  </si>
-  <si>
-    <t>Abalone, red viscera</t>
-  </si>
-  <si>
-    <t>Cultured Rock Scallop, viscera</t>
-  </si>
-  <si>
-    <t>Rock Scallop viscera</t>
-  </si>
-  <si>
-    <t>Sardine, muscle</t>
-  </si>
-  <si>
-    <t>Sardine, viscera</t>
-  </si>
-  <si>
-    <t>Sardine, whole</t>
-  </si>
-  <si>
-    <t>Sea Mussel, Sentinel</t>
-  </si>
-  <si>
-    <t>Sea Mussel, wild</t>
-  </si>
-  <si>
-    <t>Surfperch, Shiner, Meat</t>
-  </si>
-  <si>
-    <t>Surfperch, Shiner, Viscera</t>
-  </si>
-  <si>
-    <t>Lobster, Spiny, muscle</t>
-  </si>
-  <si>
-    <t>Lobster, Spiny, viscera</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>comm_name</t>
-  </si>
-  <si>
-    <t>Mixed Sea/Bay Mussels</t>
-  </si>
-  <si>
-    <t>Washington Clam, siphon</t>
-  </si>
-  <si>
-    <t>Bay Mussel, Sentinel</t>
-  </si>
-  <si>
-    <t>Clam, unidentified</t>
-  </si>
-  <si>
-    <t>Salmon, meat</t>
-  </si>
-  <si>
-    <t>Salmon, liver</t>
-  </si>
-  <si>
-    <t>Salmon, viscera</t>
-  </si>
-  <si>
-    <t>Ray, Thornback, meat</t>
-  </si>
-  <si>
-    <t>Ray, Thornback, viscera</t>
-  </si>
-  <si>
-    <t>Grunion, whole</t>
-  </si>
-  <si>
-    <t>Gooseneck Barnacle</t>
-  </si>
-  <si>
-    <t>Pismo Clam muscle</t>
-  </si>
-  <si>
-    <t>Pismo Clam viscera</t>
-  </si>
-  <si>
-    <t>Rock Scallop, wild</t>
-  </si>
-  <si>
-    <t>Sea Otter Stomach Contents</t>
-  </si>
-  <si>
-    <t>Gaper Clam siphon</t>
-  </si>
-  <si>
-    <t>Matrix spike, mussel</t>
-  </si>
-  <si>
-    <t>Rock Scallop mantle, gills</t>
-  </si>
-  <si>
-    <t>Lobster, Spiny, roe</t>
-  </si>
-  <si>
-    <t>Thornback ray</t>
-  </si>
-  <si>
-    <t>Grunion</t>
-  </si>
-  <si>
-    <t>Gooseneck barnacle</t>
-  </si>
-  <si>
-    <t>Sea otter</t>
-  </si>
-  <si>
-    <t>siphon</t>
-  </si>
-  <si>
-    <t>Salmon</t>
-  </si>
-  <si>
-    <t>liver</t>
-  </si>
-  <si>
-    <t>stomach contents</t>
-  </si>
-  <si>
-    <t>mantle/gills</t>
-  </si>
-  <si>
-    <t>roe</t>
-  </si>
-  <si>
-    <t>Clam spp.</t>
-  </si>
-  <si>
-    <t>Mussel spp.</t>
-  </si>
-  <si>
-    <t>matrix spike</t>
-  </si>
-  <si>
-    <t>Crab, Red Rock, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Dungeness, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Spider, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Brown Rock, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Pelagic Red</t>
-  </si>
-  <si>
-    <t>Pelagic Red Crab, tail</t>
-  </si>
-  <si>
-    <t>Pelagic Red Crab, head</t>
-  </si>
-  <si>
-    <t>Crab, Red Rock</t>
-  </si>
-  <si>
-    <t>Crab, unknown rock, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Yellow Rock, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Red Rock, body meat</t>
-  </si>
-  <si>
-    <t>Crab, Red Rock, leg meat</t>
-  </si>
-  <si>
-    <t>Crab, Yellow Rock, body meat</t>
-  </si>
-  <si>
-    <t>Crab, Yellow Rock, leg meat</t>
-  </si>
-  <si>
-    <t>Crab, Brown Rock, body meat</t>
-  </si>
-  <si>
-    <t>Crab, Brown Rock, leg meat</t>
-  </si>
-  <si>
-    <t>Crab, Dungeness, body meat</t>
-  </si>
-  <si>
-    <t>Crab, Dungeness, leg meat</t>
-  </si>
-  <si>
-    <t>Crab, unknown rock, body meat</t>
-  </si>
-  <si>
-    <t>Crab, Stone, viscera</t>
-  </si>
-  <si>
-    <t>Crab, Swimming</t>
-  </si>
-  <si>
-    <t>Red rock crab</t>
-  </si>
-  <si>
-    <t>Spider crab</t>
-  </si>
-  <si>
-    <t>Stone crab</t>
-  </si>
-  <si>
-    <t>Swimming crab</t>
-  </si>
-  <si>
-    <t>Rock crab</t>
-  </si>
-  <si>
-    <t>Yellow rock crab</t>
-  </si>
-  <si>
-    <t>Dungeness crab</t>
-  </si>
-  <si>
-    <t>Brown rock crab</t>
-  </si>
-  <si>
-    <t>Pelagic red crab</t>
-  </si>
-  <si>
-    <t>body meat</t>
-  </si>
-  <si>
-    <t>leg meat</t>
-  </si>
-  <si>
-    <t>tail</t>
+    <t>California (sea) mussel</t>
+  </si>
+  <si>
+    <t>Mediterranean (bay) mussel</t>
   </si>
 </sst>
 </file>
@@ -841,23 +847,23 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -868,13 +874,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
@@ -882,10 +888,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -899,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -910,10 +916,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -924,10 +930,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -938,10 +944,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -952,13 +958,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -966,13 +972,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -980,13 +986,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -994,13 +1000,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -1008,13 +1014,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -1022,13 +1028,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1036,13 +1042,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1050,13 +1056,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -1064,13 +1070,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -1078,13 +1084,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
@@ -1092,13 +1098,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -1106,13 +1112,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
         <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>32</v>
@@ -1120,13 +1126,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -1134,13 +1140,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
@@ -1148,13 +1154,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -1162,10 +1168,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1176,13 +1182,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -1190,13 +1196,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
@@ -1204,27 +1210,27 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -1232,13 +1238,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>32</v>
@@ -1246,13 +1252,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
         <v>32</v>
@@ -1260,10 +1266,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1274,41 +1280,41 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>32</v>
@@ -1316,13 +1322,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
         <v>32</v>
@@ -1330,13 +1336,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -1344,13 +1350,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
@@ -1358,13 +1364,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -1372,13 +1378,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -1386,38 +1392,38 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
         <v>32</v>
@@ -1428,13 +1434,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
         <v>32</v>
@@ -1442,13 +1448,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -1456,10 +1462,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -1470,13 +1476,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D45" t="s">
         <v>32</v>
@@ -1484,13 +1490,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D46" t="s">
         <v>32</v>
@@ -1498,13 +1504,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
         <v>32</v>
@@ -1512,13 +1518,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>146</v>
       </c>
       <c r="D48" t="s">
         <v>32</v>
@@ -1526,13 +1532,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
         <v>32</v>
@@ -1540,13 +1546,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
@@ -1554,10 +1560,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
@@ -1568,13 +1574,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D52" t="s">
         <v>32</v>
@@ -1582,13 +1588,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
         <v>32</v>
@@ -1596,13 +1602,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
         <v>32</v>
@@ -1610,13 +1616,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
@@ -1624,27 +1630,27 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>149</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
         <v>32</v>
@@ -1652,13 +1658,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>49</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
         <v>32</v>
@@ -1666,10 +1672,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
@@ -1680,13 +1686,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
@@ -1694,13 +1700,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D61" t="s">
         <v>32</v>
@@ -1708,13 +1714,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
         <v>32</v>
@@ -1722,13 +1728,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D63" t="s">
         <v>32</v>
@@ -1736,13 +1742,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="C64" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
         <v>32</v>
@@ -1750,21 +1756,21 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
         <v>33</v>
@@ -1773,18 +1779,18 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
         <v>33</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
         <v>32</v>
@@ -1792,13 +1798,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
         <v>33</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D68" t="s">
         <v>32</v>
@@ -1806,41 +1812,41 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="B69" t="s">
         <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="D70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="D71" t="s">
         <v>32</v>
@@ -1848,13 +1854,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
         <v>32</v>
@@ -1862,13 +1868,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
         <v>32</v>
@@ -1876,41 +1882,41 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="C75" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D75" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="D76" t="s">
         <v>32</v>
@@ -1918,13 +1924,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D77" t="s">
         <v>32</v>
@@ -1932,41 +1938,41 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C79" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>42</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
@@ -1974,13 +1980,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="D81" t="s">
         <v>32</v>
@@ -1988,13 +1994,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
         <v>32</v>
@@ -2002,10 +2008,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -2016,13 +2022,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="B84" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="C84" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D84" t="s">
         <v>32</v>
@@ -2030,13 +2036,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="C85" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
         <v>32</v>
@@ -2044,13 +2050,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B86" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -2058,13 +2064,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D87" t="s">
         <v>32</v>
@@ -2072,10 +2078,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="C88" t="s">
         <v>2</v>
@@ -2086,13 +2092,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="C89" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="D89" t="s">
         <v>32</v>
@@ -2100,13 +2106,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="C90" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
         <v>32</v>
@@ -2114,13 +2120,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="D91" t="s">
         <v>32</v>
@@ -2128,13 +2134,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D92" t="s">
         <v>32</v>
@@ -2142,10 +2148,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -2157,7 +2163,7 @@
   </sheetData>
   <autoFilter ref="A1:D53" xr:uid="{ED7C810D-C772-A744-9F16-FBCBA400A174}">
     <sortState ref="A2:D93">
-      <sortCondition ref="A1:A93"/>
+      <sortCondition ref="B1:B93"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>